<commit_message>
retirada a lib de consulta db
</commit_message>
<xml_diff>
--- a/posicao.xlsx
+++ b/posicao.xlsx
@@ -1684,63 +1684,63 @@
     <t>13414</t>
   </si>
   <si>
+    <t>111883</t>
+  </si>
+  <si>
+    <t>111889</t>
+  </si>
+  <si>
+    <t>1481</t>
+  </si>
+  <si>
+    <t>948</t>
+  </si>
+  <si>
+    <t>706</t>
+  </si>
+  <si>
+    <t>3737</t>
+  </si>
+  <si>
+    <t>1569</t>
+  </si>
+  <si>
+    <t>11274</t>
+  </si>
+  <si>
+    <t>111353</t>
+  </si>
+  <si>
+    <t>10899</t>
+  </si>
+  <si>
+    <t>13813</t>
+  </si>
+  <si>
+    <t>12836</t>
+  </si>
+  <si>
+    <t>13811</t>
+  </si>
+  <si>
+    <t>13022</t>
+  </si>
+  <si>
+    <t>111879</t>
+  </si>
+  <si>
+    <t>14246</t>
+  </si>
+  <si>
+    <t>10595</t>
+  </si>
+  <si>
     <t>111327</t>
   </si>
   <si>
     <t>7513</t>
   </si>
   <si>
-    <t>10899</t>
-  </si>
-  <si>
-    <t>13813</t>
-  </si>
-  <si>
-    <t>12836</t>
-  </si>
-  <si>
-    <t>13811</t>
-  </si>
-  <si>
-    <t>13022</t>
-  </si>
-  <si>
-    <t>111879</t>
-  </si>
-  <si>
-    <t>14246</t>
-  </si>
-  <si>
-    <t>10595</t>
-  </si>
-  <si>
-    <t>111883</t>
-  </si>
-  <si>
-    <t>111889</t>
-  </si>
-  <si>
-    <t>1481</t>
-  </si>
-  <si>
-    <t>948</t>
-  </si>
-  <si>
-    <t>706</t>
-  </si>
-  <si>
-    <t>3737</t>
-  </si>
-  <si>
-    <t>1569</t>
-  </si>
-  <si>
-    <t>11274</t>
-  </si>
-  <si>
-    <t>111353</t>
-  </si>
-  <si>
     <t>431</t>
   </si>
   <si>
@@ -3619,63 +3619,63 @@
     <t>225/50R18 95W P7CINT</t>
   </si>
   <si>
+    <t>235/60R16 100V RDX RXMOTION H12</t>
+  </si>
+  <si>
+    <t>275/45R20 110V ECO607</t>
+  </si>
+  <si>
+    <t>325/45R13 POTENZA 35L T9950 16L</t>
+  </si>
+  <si>
+    <t>275/80R22.5 TL 16PR 149L DIR CUL</t>
+  </si>
+  <si>
+    <t>185/55R15 WINGRO</t>
+  </si>
+  <si>
+    <t>195/45R15 CHAMPIRO 328</t>
+  </si>
+  <si>
+    <t>215/40R17 CHAMPIRO 328</t>
+  </si>
+  <si>
+    <t>245/75R16 SAVERO HT2 OWL PR10</t>
+  </si>
+  <si>
+    <t>265/65R17 HT 112S DIR TRACCIATO HT3</t>
+  </si>
+  <si>
+    <t>265/70R17 ATT771 115S</t>
+  </si>
+  <si>
+    <t>10.5/80X18 TT 10L RA45</t>
+  </si>
+  <si>
+    <t>17.5X25 TL 16(G-2/L-2) PN12</t>
+  </si>
+  <si>
+    <t>750X15 10PR CI84</t>
+  </si>
+  <si>
+    <t>245/75R16 RO-HT D PR10</t>
+  </si>
+  <si>
+    <t>205/70R15 96H RXMOTION H12</t>
+  </si>
+  <si>
+    <t>185/60R14 82H STD ATREZZO SH402</t>
+  </si>
+  <si>
+    <t>225/45R17 SN3630 94W</t>
+  </si>
+  <si>
     <t>275/80R22.5 TL 16PR 149J DIR PRO-TR</t>
   </si>
   <si>
     <t>185/60R15 84H RP18</t>
   </si>
   <si>
-    <t>265/70R17 ATT771 115S</t>
-  </si>
-  <si>
-    <t>10.5/80X18 TT 10L RA45</t>
-  </si>
-  <si>
-    <t>17.5X25 TL 16(G-2/L-2) PN12</t>
-  </si>
-  <si>
-    <t>750X15 10PR CI84</t>
-  </si>
-  <si>
-    <t>245/75R16 RO-HT D PR10</t>
-  </si>
-  <si>
-    <t>205/70R15 96H RXMOTION H12</t>
-  </si>
-  <si>
-    <t>185/60R14 82H STD ATREZZO SH402</t>
-  </si>
-  <si>
-    <t>225/45R17 SN3630 94W</t>
-  </si>
-  <si>
-    <t>235/60R16 100V RDX RXMOTION H12</t>
-  </si>
-  <si>
-    <t>275/45R20 110V ECO607</t>
-  </si>
-  <si>
-    <t>325/45R13 POTENZA 35L T9950 16L</t>
-  </si>
-  <si>
-    <t>275/80R22.5 TL 16PR 149L DIR CUL</t>
-  </si>
-  <si>
-    <t>185/55R15 WINGRO</t>
-  </si>
-  <si>
-    <t>195/45R15 CHAMPIRO 328</t>
-  </si>
-  <si>
-    <t>215/40R17 CHAMPIRO 328</t>
-  </si>
-  <si>
-    <t>245/75R16 SAVERO HT2 OWL PR10</t>
-  </si>
-  <si>
-    <t>265/65R17 HT 112S DIR TRACCIATO HT3</t>
-  </si>
-  <si>
     <t>750X16 TT 10PR 116L AT52</t>
   </si>
   <si>
@@ -4855,13 +4855,13 @@
     <t>ARMOUR</t>
   </si>
   <si>
+    <t>CHALLENGER</t>
+  </si>
+  <si>
+    <t>MAXXIS</t>
+  </si>
+  <si>
     <t>VIPAL</t>
-  </si>
-  <si>
-    <t>MAXXIS</t>
-  </si>
-  <si>
-    <t>CHALLENGER</t>
   </si>
   <si>
     <t>CHENGSHAN</t>
@@ -46933,43 +46933,40 @@
         <v>1201</v>
       </c>
       <c r="D826" t="s">
-        <v>1385</v>
+        <v>1460</v>
       </c>
       <c r="E826" t="s">
-        <v>1527</v>
+        <v>1525</v>
       </c>
       <c r="F826" t="s">
         <v>1525</v>
       </c>
       <c r="G826" t="s">
-        <v>1613</v>
+        <v>1542</v>
       </c>
       <c r="H826">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="I826">
-        <v>1080</v>
+        <v>399</v>
       </c>
       <c r="J826">
-        <v>1080</v>
+        <v>279.3</v>
       </c>
       <c r="K826">
-        <v>1382</v>
+        <v>511</v>
       </c>
       <c r="L826">
         <v>0.2188</v>
       </c>
       <c r="M826" t="s">
-        <v>1697</v>
-      </c>
-      <c r="N826" t="s">
-        <v>1759</v>
+        <v>1727</v>
       </c>
       <c r="O826">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="P826">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="827" spans="1:16">
@@ -46983,7 +46980,7 @@
         <v>1202</v>
       </c>
       <c r="D827" t="s">
-        <v>1356</v>
+        <v>1494</v>
       </c>
       <c r="E827" t="s">
         <v>1525</v>
@@ -46992,31 +46989,34 @@
         <v>1525</v>
       </c>
       <c r="G827" t="s">
-        <v>1566</v>
+        <v>1542</v>
       </c>
       <c r="H827">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I827">
-        <v>269</v>
+        <v>800</v>
       </c>
       <c r="J827">
-        <v>188.3</v>
+        <v>800</v>
       </c>
       <c r="K827">
-        <v>328</v>
+        <v>1024</v>
       </c>
       <c r="L827">
-        <v>0.1803</v>
+        <v>0.2188</v>
       </c>
       <c r="M827" t="s">
-        <v>1727</v>
+        <v>1645</v>
+      </c>
+      <c r="N827" t="s">
+        <v>1697</v>
       </c>
       <c r="O827">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="P827">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="828" spans="1:16">
@@ -47024,43 +47024,46 @@
         <v>23</v>
       </c>
       <c r="B828" t="s">
-        <v>510</v>
+        <v>134</v>
       </c>
       <c r="C828" t="s">
-        <v>1155</v>
+        <v>787</v>
       </c>
       <c r="D828" t="s">
-        <v>1486</v>
+        <v>1382</v>
       </c>
       <c r="E828" t="s">
-        <v>1525</v>
+        <v>1535</v>
       </c>
       <c r="F828" t="s">
-        <v>1525</v>
+        <v>1541</v>
       </c>
       <c r="G828" t="s">
-        <v>1566</v>
+        <v>1569</v>
       </c>
       <c r="H828">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="I828">
-        <v>407</v>
+        <v>1772</v>
       </c>
       <c r="J828">
-        <v>284.89</v>
+        <v>1240.45</v>
       </c>
       <c r="K828">
-        <v>485</v>
+        <v>2091</v>
       </c>
       <c r="L828">
-        <v>0.1609</v>
+        <v>0.1525</v>
       </c>
       <c r="M828" t="s">
         <v>1727</v>
       </c>
+      <c r="N828" t="s">
+        <v>1687</v>
+      </c>
       <c r="O828">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="P828">
         <v>16</v>
@@ -47077,7 +47080,7 @@
         <v>1203</v>
       </c>
       <c r="D829" t="s">
-        <v>1373</v>
+        <v>1497</v>
       </c>
       <c r="E829" t="s">
         <v>1525</v>
@@ -47086,19 +47089,19 @@
         <v>1525</v>
       </c>
       <c r="G829" t="s">
-        <v>1614</v>
+        <v>1570</v>
       </c>
       <c r="H829">
         <v>1</v>
       </c>
       <c r="I829">
-        <v>572</v>
+        <v>821</v>
       </c>
       <c r="J829">
-        <v>400.56</v>
+        <v>574.95</v>
       </c>
       <c r="K829">
-        <v>682</v>
+        <v>979</v>
       </c>
       <c r="L829">
         <v>0.1609</v>
@@ -47118,46 +47121,49 @@
         <v>23</v>
       </c>
       <c r="B830" t="s">
-        <v>559</v>
+        <v>143</v>
       </c>
       <c r="C830" t="s">
-        <v>1204</v>
+        <v>796</v>
       </c>
       <c r="D830" t="s">
-        <v>1406</v>
+        <v>1385</v>
       </c>
       <c r="E830" t="s">
-        <v>1539</v>
+        <v>1527</v>
       </c>
       <c r="F830" t="s">
-        <v>1539</v>
+        <v>1525</v>
       </c>
       <c r="G830" t="s">
-        <v>1557</v>
+        <v>1571</v>
       </c>
       <c r="H830">
-        <v>3</v>
+        <v>246</v>
       </c>
       <c r="I830">
-        <v>1084</v>
+        <v>1461</v>
       </c>
       <c r="J830">
-        <v>758.51</v>
+        <v>0</v>
       </c>
       <c r="K830">
-        <v>1262</v>
+        <v>1870</v>
       </c>
       <c r="L830">
-        <v>0.1416</v>
+        <v>0.2187</v>
       </c>
       <c r="M830" t="s">
-        <v>1727</v>
+        <v>1645</v>
+      </c>
+      <c r="N830" t="s">
+        <v>1759</v>
       </c>
       <c r="O830">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="P830">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="831" spans="1:16">
@@ -47165,37 +47171,37 @@
         <v>23</v>
       </c>
       <c r="B831" t="s">
-        <v>219</v>
+        <v>559</v>
       </c>
       <c r="C831" t="s">
-        <v>870</v>
+        <v>1204</v>
       </c>
       <c r="D831" t="s">
-        <v>1406</v>
+        <v>1385</v>
       </c>
       <c r="E831" t="s">
-        <v>1539</v>
+        <v>1527</v>
       </c>
       <c r="F831" t="s">
-        <v>1539</v>
+        <v>1525</v>
       </c>
       <c r="G831" t="s">
-        <v>1557</v>
+        <v>1613</v>
       </c>
       <c r="H831">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I831">
-        <v>1203</v>
+        <v>1968</v>
       </c>
       <c r="J831">
-        <v>841.92</v>
+        <v>1377.25</v>
       </c>
       <c r="K831">
-        <v>1401</v>
+        <v>2400</v>
       </c>
       <c r="L831">
-        <v>0.1416</v>
+        <v>0.1803</v>
       </c>
       <c r="M831" t="s">
         <v>1727</v>
@@ -47212,46 +47218,43 @@
         <v>23</v>
       </c>
       <c r="B832" t="s">
-        <v>136</v>
+        <v>289</v>
       </c>
       <c r="C832" t="s">
-        <v>789</v>
+        <v>938</v>
       </c>
       <c r="D832" t="s">
-        <v>1384</v>
+        <v>1382</v>
       </c>
       <c r="E832" t="s">
-        <v>1528</v>
+        <v>1535</v>
       </c>
       <c r="F832" t="s">
-        <v>1528</v>
+        <v>1541</v>
       </c>
       <c r="G832" t="s">
-        <v>1557</v>
+        <v>1546</v>
       </c>
       <c r="H832">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I832">
-        <v>1463</v>
+        <v>2285</v>
       </c>
       <c r="J832">
-        <v>1024.3</v>
+        <v>1599.74</v>
       </c>
       <c r="K832">
-        <v>1705</v>
+        <v>2654</v>
       </c>
       <c r="L832">
-        <v>0.1416</v>
+        <v>0.139</v>
       </c>
       <c r="M832" t="s">
         <v>1727</v>
       </c>
-      <c r="N832" t="s">
-        <v>1759</v>
-      </c>
       <c r="O832">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="P832">
         <v>16</v>
@@ -47268,31 +47271,31 @@
         <v>1205</v>
       </c>
       <c r="D833" t="s">
-        <v>1417</v>
+        <v>1379</v>
       </c>
       <c r="E833" t="s">
-        <v>1538</v>
+        <v>1525</v>
       </c>
       <c r="F833" t="s">
-        <v>1538</v>
+        <v>1525</v>
       </c>
       <c r="G833" t="s">
-        <v>1557</v>
+        <v>1548</v>
       </c>
       <c r="H833">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I833">
-        <v>5029</v>
+        <v>279</v>
       </c>
       <c r="J833">
-        <v>3520.27</v>
+        <v>194.96</v>
       </c>
       <c r="K833">
-        <v>5859</v>
+        <v>332</v>
       </c>
       <c r="L833">
-        <v>0.1416</v>
+        <v>0.1609</v>
       </c>
       <c r="M833" t="s">
         <v>1727</v>
@@ -47309,46 +47312,46 @@
         <v>23</v>
       </c>
       <c r="B834" t="s">
-        <v>236</v>
+        <v>561</v>
       </c>
       <c r="C834" t="s">
-        <v>749</v>
+        <v>1206</v>
       </c>
       <c r="D834" t="s">
-        <v>1345</v>
+        <v>1498</v>
       </c>
       <c r="E834" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
       <c r="F834" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
       <c r="G834" t="s">
-        <v>1557</v>
+        <v>1548</v>
       </c>
       <c r="H834">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="I834">
-        <v>387</v>
+        <v>310</v>
       </c>
       <c r="J834">
-        <v>270.98</v>
+        <v>0</v>
       </c>
       <c r="K834">
-        <v>461</v>
+        <v>370</v>
       </c>
       <c r="L834">
         <v>0.1609</v>
       </c>
       <c r="M834" t="s">
-        <v>1727</v>
+        <v>1697</v>
       </c>
       <c r="O834">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="P834">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="835" spans="1:16">
@@ -47356,46 +47359,46 @@
         <v>23</v>
       </c>
       <c r="B835" t="s">
-        <v>82</v>
+        <v>292</v>
       </c>
       <c r="C835" t="s">
-        <v>735</v>
+        <v>941</v>
       </c>
       <c r="D835" t="s">
-        <v>1369</v>
+        <v>1436</v>
       </c>
       <c r="E835" t="s">
-        <v>1529</v>
+        <v>1525</v>
       </c>
       <c r="F835" t="s">
-        <v>1529</v>
+        <v>1525</v>
       </c>
       <c r="G835" t="s">
-        <v>1557</v>
+        <v>1548</v>
       </c>
       <c r="H835">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="I835">
-        <v>622</v>
+        <v>445</v>
       </c>
       <c r="J835">
-        <v>435.62</v>
+        <v>1225</v>
       </c>
       <c r="K835">
-        <v>742</v>
+        <v>531</v>
       </c>
       <c r="L835">
         <v>0.1609</v>
       </c>
       <c r="M835" t="s">
-        <v>1727</v>
+        <v>1697</v>
       </c>
       <c r="O835">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="P835">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="836" spans="1:16">
@@ -47403,49 +47406,46 @@
         <v>23</v>
       </c>
       <c r="B836" t="s">
-        <v>106</v>
+        <v>562</v>
       </c>
       <c r="C836" t="s">
-        <v>759</v>
+        <v>1207</v>
       </c>
       <c r="D836" t="s">
-        <v>1376</v>
+        <v>1499</v>
       </c>
       <c r="E836" t="s">
-        <v>1533</v>
+        <v>1525</v>
       </c>
       <c r="F836" t="s">
-        <v>1533</v>
+        <v>1525</v>
       </c>
       <c r="G836" t="s">
-        <v>1557</v>
+        <v>1548</v>
       </c>
       <c r="H836">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I836">
-        <v>528</v>
+        <v>380</v>
       </c>
       <c r="J836">
-        <v>0</v>
+        <v>265.69</v>
       </c>
       <c r="K836">
-        <v>629</v>
+        <v>452</v>
       </c>
       <c r="L836">
         <v>0.1609</v>
       </c>
       <c r="M836" t="s">
-        <v>1697</v>
-      </c>
-      <c r="N836" t="s">
-        <v>1759</v>
+        <v>1727</v>
       </c>
       <c r="O836">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="P836">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="837" spans="1:16">
@@ -47453,37 +47453,37 @@
         <v>23</v>
       </c>
       <c r="B837" t="s">
-        <v>485</v>
+        <v>563</v>
       </c>
       <c r="C837" t="s">
-        <v>1132</v>
+        <v>1208</v>
       </c>
       <c r="D837" t="s">
-        <v>1485</v>
+        <v>1439</v>
       </c>
       <c r="E837" t="s">
-        <v>1535</v>
+        <v>1525</v>
       </c>
       <c r="F837" t="s">
-        <v>1541</v>
+        <v>1525</v>
       </c>
       <c r="G837" t="s">
-        <v>1557</v>
+        <v>1548</v>
       </c>
       <c r="H837">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="I837">
-        <v>2352</v>
+        <v>519</v>
       </c>
       <c r="J837">
-        <v>1646.21</v>
+        <v>363.49</v>
       </c>
       <c r="K837">
-        <v>2775</v>
+        <v>619</v>
       </c>
       <c r="L837">
-        <v>0.1525</v>
+        <v>0.1609</v>
       </c>
       <c r="M837" t="s">
         <v>1727</v>
@@ -47500,46 +47500,46 @@
         <v>23</v>
       </c>
       <c r="B838" t="s">
-        <v>489</v>
+        <v>564</v>
       </c>
       <c r="C838" t="s">
-        <v>858</v>
+        <v>1209</v>
       </c>
       <c r="D838" t="s">
-        <v>1382</v>
+        <v>1341</v>
       </c>
       <c r="E838" t="s">
-        <v>1535</v>
+        <v>1525</v>
       </c>
       <c r="F838" t="s">
-        <v>1541</v>
+        <v>1525</v>
       </c>
       <c r="G838" t="s">
-        <v>1557</v>
+        <v>1553</v>
       </c>
       <c r="H838">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="I838">
-        <v>2558</v>
+        <v>580</v>
       </c>
       <c r="J838">
-        <v>1790.88</v>
+        <v>0</v>
       </c>
       <c r="K838">
-        <v>2967</v>
+        <v>742</v>
       </c>
       <c r="L838">
-        <v>0.1377</v>
+        <v>0.2188</v>
       </c>
       <c r="M838" t="s">
-        <v>1727</v>
+        <v>1697</v>
       </c>
       <c r="O838">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="P838">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="839" spans="1:16">
@@ -47547,37 +47547,37 @@
         <v>23</v>
       </c>
       <c r="B839" t="s">
-        <v>561</v>
+        <v>565</v>
       </c>
       <c r="C839" t="s">
-        <v>1206</v>
+        <v>1210</v>
       </c>
       <c r="D839" t="s">
-        <v>1474</v>
+        <v>1373</v>
       </c>
       <c r="E839" t="s">
-        <v>1537</v>
+        <v>1525</v>
       </c>
       <c r="F839" t="s">
-        <v>1537</v>
+        <v>1525</v>
       </c>
       <c r="G839" t="s">
-        <v>1557</v>
+        <v>1614</v>
       </c>
       <c r="H839">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I839">
-        <v>1303</v>
+        <v>572</v>
       </c>
       <c r="J839">
-        <v>912.16</v>
+        <v>400.56</v>
       </c>
       <c r="K839">
-        <v>1518</v>
+        <v>682</v>
       </c>
       <c r="L839">
-        <v>0.1416</v>
+        <v>0.1609</v>
       </c>
       <c r="M839" t="s">
         <v>1727</v>
@@ -47594,37 +47594,37 @@
         <v>23</v>
       </c>
       <c r="B840" t="s">
-        <v>562</v>
+        <v>566</v>
       </c>
       <c r="C840" t="s">
-        <v>1207</v>
+        <v>1211</v>
       </c>
       <c r="D840" t="s">
-        <v>1439</v>
+        <v>1406</v>
       </c>
       <c r="E840" t="s">
-        <v>1525</v>
+        <v>1539</v>
       </c>
       <c r="F840" t="s">
-        <v>1525</v>
+        <v>1539</v>
       </c>
       <c r="G840" t="s">
-        <v>1559</v>
+        <v>1557</v>
       </c>
       <c r="H840">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I840">
-        <v>591</v>
+        <v>1084</v>
       </c>
       <c r="J840">
-        <v>414</v>
+        <v>758.51</v>
       </c>
       <c r="K840">
-        <v>705</v>
+        <v>1262</v>
       </c>
       <c r="L840">
-        <v>0.1609</v>
+        <v>0.1416</v>
       </c>
       <c r="M840" t="s">
         <v>1727</v>
@@ -47641,37 +47641,37 @@
         <v>23</v>
       </c>
       <c r="B841" t="s">
-        <v>563</v>
+        <v>219</v>
       </c>
       <c r="C841" t="s">
-        <v>1208</v>
+        <v>870</v>
       </c>
       <c r="D841" t="s">
-        <v>1340</v>
+        <v>1406</v>
       </c>
       <c r="E841" t="s">
-        <v>1525</v>
+        <v>1539</v>
       </c>
       <c r="F841" t="s">
-        <v>1525</v>
+        <v>1539</v>
       </c>
       <c r="G841" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="H841">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I841">
-        <v>340</v>
+        <v>1203</v>
       </c>
       <c r="J841">
-        <v>238</v>
+        <v>841.92</v>
       </c>
       <c r="K841">
-        <v>435</v>
+        <v>1401</v>
       </c>
       <c r="L841">
-        <v>0.2188</v>
+        <v>0.1416</v>
       </c>
       <c r="M841" t="s">
         <v>1727</v>
@@ -47688,43 +47688,46 @@
         <v>23</v>
       </c>
       <c r="B842" t="s">
-        <v>564</v>
+        <v>136</v>
       </c>
       <c r="C842" t="s">
-        <v>1209</v>
+        <v>789</v>
       </c>
       <c r="D842" t="s">
-        <v>1400</v>
+        <v>1384</v>
       </c>
       <c r="E842" t="s">
-        <v>1525</v>
+        <v>1528</v>
       </c>
       <c r="F842" t="s">
-        <v>1525</v>
+        <v>1528</v>
       </c>
       <c r="G842" t="s">
-        <v>1587</v>
+        <v>1557</v>
       </c>
       <c r="H842">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I842">
-        <v>142</v>
+        <v>1463</v>
       </c>
       <c r="J842">
-        <v>99.69</v>
+        <v>1024.3</v>
       </c>
       <c r="K842">
-        <v>170</v>
+        <v>1705</v>
       </c>
       <c r="L842">
-        <v>0.1609</v>
+        <v>0.1416</v>
       </c>
       <c r="M842" t="s">
         <v>1727</v>
       </c>
+      <c r="N842" t="s">
+        <v>1759</v>
+      </c>
       <c r="O842">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="P842">
         <v>16</v>
@@ -47735,37 +47738,37 @@
         <v>23</v>
       </c>
       <c r="B843" t="s">
-        <v>252</v>
+        <v>567</v>
       </c>
       <c r="C843" t="s">
-        <v>901</v>
+        <v>1212</v>
       </c>
       <c r="D843" t="s">
-        <v>1382</v>
+        <v>1417</v>
       </c>
       <c r="E843" t="s">
-        <v>1535</v>
+        <v>1538</v>
       </c>
       <c r="F843" t="s">
-        <v>1541</v>
+        <v>1538</v>
       </c>
       <c r="G843" t="s">
-        <v>1588</v>
+        <v>1557</v>
       </c>
       <c r="H843">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="I843">
-        <v>2061</v>
+        <v>5029</v>
       </c>
       <c r="J843">
-        <v>1442.46</v>
+        <v>3520.27</v>
       </c>
       <c r="K843">
-        <v>2432</v>
+        <v>5859</v>
       </c>
       <c r="L843">
-        <v>0.1525</v>
+        <v>0.1416</v>
       </c>
       <c r="M843" t="s">
         <v>1727</v>
@@ -47782,34 +47785,34 @@
         <v>23</v>
       </c>
       <c r="B844" t="s">
-        <v>565</v>
+        <v>236</v>
       </c>
       <c r="C844" t="s">
-        <v>1210</v>
+        <v>749</v>
       </c>
       <c r="D844" t="s">
-        <v>1376</v>
+        <v>1345</v>
       </c>
       <c r="E844" t="s">
-        <v>1525</v>
+        <v>1526</v>
       </c>
       <c r="F844" t="s">
-        <v>1525</v>
+        <v>1526</v>
       </c>
       <c r="G844" t="s">
-        <v>1609</v>
+        <v>1557</v>
       </c>
       <c r="H844">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="I844">
-        <v>350</v>
+        <v>387</v>
       </c>
       <c r="J844">
-        <v>245.31</v>
+        <v>270.98</v>
       </c>
       <c r="K844">
-        <v>418</v>
+        <v>461</v>
       </c>
       <c r="L844">
         <v>0.1609</v>
@@ -47829,37 +47832,37 @@
         <v>23</v>
       </c>
       <c r="B845" t="s">
-        <v>566</v>
+        <v>82</v>
       </c>
       <c r="C845" t="s">
-        <v>1211</v>
+        <v>735</v>
       </c>
       <c r="D845" t="s">
-        <v>1460</v>
+        <v>1369</v>
       </c>
       <c r="E845" t="s">
-        <v>1525</v>
+        <v>1529</v>
       </c>
       <c r="F845" t="s">
-        <v>1525</v>
+        <v>1529</v>
       </c>
       <c r="G845" t="s">
-        <v>1542</v>
+        <v>1557</v>
       </c>
       <c r="H845">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="I845">
-        <v>399</v>
+        <v>622</v>
       </c>
       <c r="J845">
-        <v>279.3</v>
+        <v>435.62</v>
       </c>
       <c r="K845">
-        <v>511</v>
+        <v>742</v>
       </c>
       <c r="L845">
-        <v>0.2188</v>
+        <v>0.1609</v>
       </c>
       <c r="M845" t="s">
         <v>1727</v>
@@ -47876,49 +47879,49 @@
         <v>23</v>
       </c>
       <c r="B846" t="s">
-        <v>567</v>
+        <v>106</v>
       </c>
       <c r="C846" t="s">
-        <v>1212</v>
+        <v>759</v>
       </c>
       <c r="D846" t="s">
-        <v>1494</v>
+        <v>1376</v>
       </c>
       <c r="E846" t="s">
-        <v>1525</v>
+        <v>1533</v>
       </c>
       <c r="F846" t="s">
-        <v>1525</v>
+        <v>1533</v>
       </c>
       <c r="G846" t="s">
-        <v>1542</v>
+        <v>1557</v>
       </c>
       <c r="H846">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I846">
-        <v>800</v>
+        <v>528</v>
       </c>
       <c r="J846">
-        <v>800</v>
+        <v>0</v>
       </c>
       <c r="K846">
-        <v>1024</v>
+        <v>629</v>
       </c>
       <c r="L846">
-        <v>0.2188</v>
+        <v>0.1609</v>
       </c>
       <c r="M846" t="s">
-        <v>1645</v>
+        <v>1697</v>
       </c>
       <c r="N846" t="s">
-        <v>1697</v>
+        <v>1759</v>
       </c>
       <c r="O846">
+        <v>2</v>
+      </c>
+      <c r="P846">
         <v>14</v>
-      </c>
-      <c r="P846">
-        <v>9</v>
       </c>
     </row>
     <row r="847" spans="1:16">
@@ -47926,13 +47929,13 @@
         <v>23</v>
       </c>
       <c r="B847" t="s">
-        <v>134</v>
+        <v>485</v>
       </c>
       <c r="C847" t="s">
-        <v>787</v>
+        <v>1132</v>
       </c>
       <c r="D847" t="s">
-        <v>1382</v>
+        <v>1485</v>
       </c>
       <c r="E847" t="s">
         <v>1535</v>
@@ -47941,19 +47944,19 @@
         <v>1541</v>
       </c>
       <c r="G847" t="s">
-        <v>1569</v>
+        <v>1557</v>
       </c>
       <c r="H847">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="I847">
-        <v>1772</v>
+        <v>2352</v>
       </c>
       <c r="J847">
-        <v>1240.45</v>
+        <v>1646.21</v>
       </c>
       <c r="K847">
-        <v>2091</v>
+        <v>2775</v>
       </c>
       <c r="L847">
         <v>0.1525</v>
@@ -47961,11 +47964,8 @@
       <c r="M847" t="s">
         <v>1727</v>
       </c>
-      <c r="N847" t="s">
-        <v>1687</v>
-      </c>
       <c r="O847">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="P847">
         <v>16</v>
@@ -47976,37 +47976,37 @@
         <v>23</v>
       </c>
       <c r="B848" t="s">
-        <v>568</v>
+        <v>489</v>
       </c>
       <c r="C848" t="s">
-        <v>1213</v>
+        <v>858</v>
       </c>
       <c r="D848" t="s">
-        <v>1497</v>
+        <v>1382</v>
       </c>
       <c r="E848" t="s">
-        <v>1525</v>
+        <v>1535</v>
       </c>
       <c r="F848" t="s">
-        <v>1525</v>
+        <v>1541</v>
       </c>
       <c r="G848" t="s">
-        <v>1570</v>
+        <v>1557</v>
       </c>
       <c r="H848">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="I848">
-        <v>821</v>
+        <v>2558</v>
       </c>
       <c r="J848">
-        <v>574.95</v>
+        <v>1790.88</v>
       </c>
       <c r="K848">
-        <v>979</v>
+        <v>2967</v>
       </c>
       <c r="L848">
-        <v>0.1609</v>
+        <v>0.1377</v>
       </c>
       <c r="M848" t="s">
         <v>1727</v>
@@ -48023,49 +48023,46 @@
         <v>23</v>
       </c>
       <c r="B849" t="s">
-        <v>143</v>
+        <v>568</v>
       </c>
       <c r="C849" t="s">
-        <v>796</v>
+        <v>1213</v>
       </c>
       <c r="D849" t="s">
-        <v>1385</v>
+        <v>1474</v>
       </c>
       <c r="E849" t="s">
-        <v>1527</v>
+        <v>1537</v>
       </c>
       <c r="F849" t="s">
-        <v>1525</v>
+        <v>1537</v>
       </c>
       <c r="G849" t="s">
-        <v>1571</v>
+        <v>1557</v>
       </c>
       <c r="H849">
-        <v>246</v>
+        <v>4</v>
       </c>
       <c r="I849">
-        <v>1461</v>
+        <v>1303</v>
       </c>
       <c r="J849">
-        <v>0</v>
+        <v>912.16</v>
       </c>
       <c r="K849">
-        <v>1870</v>
+        <v>1518</v>
       </c>
       <c r="L849">
-        <v>0.2187</v>
+        <v>0.1416</v>
       </c>
       <c r="M849" t="s">
-        <v>1645</v>
-      </c>
-      <c r="N849" t="s">
-        <v>1759</v>
+        <v>1727</v>
       </c>
       <c r="O849">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="P849">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="850" spans="1:16">
@@ -48079,31 +48076,31 @@
         <v>1214</v>
       </c>
       <c r="D850" t="s">
-        <v>1385</v>
+        <v>1439</v>
       </c>
       <c r="E850" t="s">
-        <v>1527</v>
+        <v>1525</v>
       </c>
       <c r="F850" t="s">
         <v>1525</v>
       </c>
       <c r="G850" t="s">
-        <v>1615</v>
+        <v>1559</v>
       </c>
       <c r="H850">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I850">
-        <v>1968</v>
+        <v>591</v>
       </c>
       <c r="J850">
-        <v>1377.25</v>
+        <v>414</v>
       </c>
       <c r="K850">
-        <v>2400</v>
+        <v>705</v>
       </c>
       <c r="L850">
-        <v>0.1803</v>
+        <v>0.1609</v>
       </c>
       <c r="M850" t="s">
         <v>1727</v>
@@ -48120,37 +48117,37 @@
         <v>23</v>
       </c>
       <c r="B851" t="s">
-        <v>289</v>
+        <v>570</v>
       </c>
       <c r="C851" t="s">
-        <v>938</v>
+        <v>1215</v>
       </c>
       <c r="D851" t="s">
-        <v>1382</v>
+        <v>1340</v>
       </c>
       <c r="E851" t="s">
-        <v>1535</v>
+        <v>1525</v>
       </c>
       <c r="F851" t="s">
-        <v>1541</v>
+        <v>1525</v>
       </c>
       <c r="G851" t="s">
-        <v>1546</v>
+        <v>1558</v>
       </c>
       <c r="H851">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I851">
-        <v>2285</v>
+        <v>340</v>
       </c>
       <c r="J851">
-        <v>1599.74</v>
+        <v>238</v>
       </c>
       <c r="K851">
-        <v>2654</v>
+        <v>435</v>
       </c>
       <c r="L851">
-        <v>0.139</v>
+        <v>0.2188</v>
       </c>
       <c r="M851" t="s">
         <v>1727</v>
@@ -48167,13 +48164,13 @@
         <v>23</v>
       </c>
       <c r="B852" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="C852" t="s">
-        <v>1215</v>
+        <v>1216</v>
       </c>
       <c r="D852" t="s">
-        <v>1379</v>
+        <v>1400</v>
       </c>
       <c r="E852" t="s">
         <v>1525</v>
@@ -48182,19 +48179,19 @@
         <v>1525</v>
       </c>
       <c r="G852" t="s">
-        <v>1548</v>
+        <v>1587</v>
       </c>
       <c r="H852">
         <v>1</v>
       </c>
       <c r="I852">
-        <v>279</v>
+        <v>142</v>
       </c>
       <c r="J852">
-        <v>194.96</v>
+        <v>99.69</v>
       </c>
       <c r="K852">
-        <v>332</v>
+        <v>170</v>
       </c>
       <c r="L852">
         <v>0.1609</v>
@@ -48214,46 +48211,46 @@
         <v>23</v>
       </c>
       <c r="B853" t="s">
-        <v>571</v>
+        <v>252</v>
       </c>
       <c r="C853" t="s">
-        <v>1216</v>
+        <v>901</v>
       </c>
       <c r="D853" t="s">
-        <v>1498</v>
+        <v>1382</v>
       </c>
       <c r="E853" t="s">
-        <v>1525</v>
+        <v>1535</v>
       </c>
       <c r="F853" t="s">
-        <v>1525</v>
+        <v>1541</v>
       </c>
       <c r="G853" t="s">
-        <v>1548</v>
+        <v>1588</v>
       </c>
       <c r="H853">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="I853">
-        <v>310</v>
+        <v>2061</v>
       </c>
       <c r="J853">
-        <v>0</v>
+        <v>1442.46</v>
       </c>
       <c r="K853">
-        <v>370</v>
+        <v>2432</v>
       </c>
       <c r="L853">
-        <v>0.1609</v>
+        <v>0.1525</v>
       </c>
       <c r="M853" t="s">
-        <v>1697</v>
+        <v>1727</v>
       </c>
       <c r="O853">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="P853">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="854" spans="1:16">
@@ -48261,13 +48258,13 @@
         <v>23</v>
       </c>
       <c r="B854" t="s">
-        <v>292</v>
+        <v>572</v>
       </c>
       <c r="C854" t="s">
-        <v>941</v>
+        <v>1217</v>
       </c>
       <c r="D854" t="s">
-        <v>1436</v>
+        <v>1376</v>
       </c>
       <c r="E854" t="s">
         <v>1525</v>
@@ -48276,31 +48273,31 @@
         <v>1525</v>
       </c>
       <c r="G854" t="s">
-        <v>1548</v>
+        <v>1609</v>
       </c>
       <c r="H854">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I854">
-        <v>445</v>
+        <v>350</v>
       </c>
       <c r="J854">
-        <v>1225</v>
+        <v>245.31</v>
       </c>
       <c r="K854">
-        <v>531</v>
+        <v>418</v>
       </c>
       <c r="L854">
         <v>0.1609</v>
       </c>
       <c r="M854" t="s">
-        <v>1697</v>
+        <v>1727</v>
       </c>
       <c r="O854">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="P854">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="855" spans="1:16">
@@ -48308,46 +48305,49 @@
         <v>23</v>
       </c>
       <c r="B855" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="C855" t="s">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="D855" t="s">
-        <v>1499</v>
+        <v>1385</v>
       </c>
       <c r="E855" t="s">
-        <v>1525</v>
+        <v>1527</v>
       </c>
       <c r="F855" t="s">
         <v>1525</v>
       </c>
       <c r="G855" t="s">
-        <v>1548</v>
+        <v>1615</v>
       </c>
       <c r="H855">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="I855">
-        <v>380</v>
+        <v>1080</v>
       </c>
       <c r="J855">
-        <v>265.69</v>
+        <v>1080</v>
       </c>
       <c r="K855">
-        <v>452</v>
+        <v>1382</v>
       </c>
       <c r="L855">
-        <v>0.1609</v>
+        <v>0.2188</v>
       </c>
       <c r="M855" t="s">
-        <v>1727</v>
+        <v>1697</v>
+      </c>
+      <c r="N855" t="s">
+        <v>1759</v>
       </c>
       <c r="O855">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="P855">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="856" spans="1:16">
@@ -48355,13 +48355,13 @@
         <v>23</v>
       </c>
       <c r="B856" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="C856" t="s">
-        <v>1218</v>
+        <v>1219</v>
       </c>
       <c r="D856" t="s">
-        <v>1439</v>
+        <v>1356</v>
       </c>
       <c r="E856" t="s">
         <v>1525</v>
@@ -48370,22 +48370,22 @@
         <v>1525</v>
       </c>
       <c r="G856" t="s">
-        <v>1548</v>
+        <v>1566</v>
       </c>
       <c r="H856">
         <v>1</v>
       </c>
       <c r="I856">
-        <v>519</v>
+        <v>269</v>
       </c>
       <c r="J856">
-        <v>363.49</v>
+        <v>188.3</v>
       </c>
       <c r="K856">
-        <v>619</v>
+        <v>328</v>
       </c>
       <c r="L856">
-        <v>0.1609</v>
+        <v>0.1803</v>
       </c>
       <c r="M856" t="s">
         <v>1727</v>
@@ -48402,13 +48402,13 @@
         <v>23</v>
       </c>
       <c r="B857" t="s">
-        <v>574</v>
+        <v>510</v>
       </c>
       <c r="C857" t="s">
-        <v>1219</v>
+        <v>1155</v>
       </c>
       <c r="D857" t="s">
-        <v>1341</v>
+        <v>1486</v>
       </c>
       <c r="E857" t="s">
         <v>1525</v>
@@ -48417,31 +48417,31 @@
         <v>1525</v>
       </c>
       <c r="G857" t="s">
-        <v>1553</v>
+        <v>1566</v>
       </c>
       <c r="H857">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I857">
-        <v>580</v>
+        <v>407</v>
       </c>
       <c r="J857">
-        <v>0</v>
+        <v>284.89</v>
       </c>
       <c r="K857">
-        <v>742</v>
+        <v>485</v>
       </c>
       <c r="L857">
-        <v>0.2188</v>
+        <v>0.1609</v>
       </c>
       <c r="M857" t="s">
-        <v>1697</v>
+        <v>1727</v>
       </c>
       <c r="O857">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="P857">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="858" spans="1:16">

</xml_diff>